<commit_message>
Some more progress in framework
</commit_message>
<xml_diff>
--- a/CoreFramework1/src/main/java/com/rupjit/automationqa/data/A suite.xlsx
+++ b/CoreFramework1/src/main/java/com/rupjit/automationqa/data/A suite.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
+    <workbookView windowWidth="14925" windowHeight="5955"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Testcases" sheetId="1" r:id="rId1"/>
     <sheet name="TestCase_A1" sheetId="2" r:id="rId2"/>
     <sheet name="TestCase_A2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:H9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
-  <si>
-    <t>TCID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+  <si>
+    <t>TCName</t>
   </si>
   <si>
     <t>Description</t>
@@ -27,40 +28,43 @@
     <t>Runmode</t>
   </si>
   <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>TestCase A1</t>
+  </si>
+  <si>
+    <t>Description for Testcase A1</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>TestCase A2</t>
+  </si>
+  <si>
+    <t>Description for Testcase A2</t>
+  </si>
+  <si>
+    <t>DataA1_1</t>
+  </si>
+  <si>
+    <t>DataA1_2</t>
+  </si>
+  <si>
+    <t>DataA1_3</t>
+  </si>
+  <si>
+    <t>DataA1_4</t>
+  </si>
+  <si>
+    <t>DataA1_5</t>
+  </si>
+  <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>TestCase A1</t>
-  </si>
-  <si>
-    <t>Description for Testcase A1</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>TestCase A2</t>
-  </si>
-  <si>
-    <t>Description for Testcase A2</t>
-  </si>
-  <si>
-    <t>DataA1_1</t>
-  </si>
-  <si>
-    <t>DataA1_2</t>
-  </si>
-  <si>
-    <t>DataA1_3</t>
-  </si>
-  <si>
-    <t>DataA1_4</t>
-  </si>
-  <si>
-    <t>DataA1_5</t>
   </si>
   <si>
     <t>Error</t>
@@ -87,11 +91,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,38 +104,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -143,17 +120,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,45 +220,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,7 +235,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,31 +247,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,187 +263,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,6 +508,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -538,15 +549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -561,162 +563,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1045,8 +1036,8 @@
   <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1106,7 +1097,7 @@
   <sheetPr/>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1140,10 +1131,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1245,23 +1236,23 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7">

</xml_diff>

<commit_message>
Core Data Driven Framework with POM design is complete
</commit_message>
<xml_diff>
--- a/CoreFramework1/src/main/java/com/rupjit/automationqa/data/A suite.xlsx
+++ b/CoreFramework1/src/main/java/com/rupjit/automationqa/data/A suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14925" windowHeight="5955"/>
+    <workbookView windowWidth="13980" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
   <si>
     <t>TCName</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Results</t>
   </si>
   <si>
-    <t>TestCase A1</t>
+    <t>TestCase_A1</t>
   </si>
   <si>
     <t>Description for Testcase A1</t>
@@ -40,15 +40,15 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>TestCase A2</t>
+    <t>TestCase_A2</t>
   </si>
   <si>
     <t>Description for Testcase A2</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>DataA1_1</t>
   </si>
   <si>
@@ -64,12 +64,63 @@
     <t>DataA1_5</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
+    <t>dataA1_1_1</t>
+  </si>
+  <si>
+    <t>dataA1_1_2</t>
+  </si>
+  <si>
+    <t>dataA1_1_3</t>
+  </si>
+  <si>
+    <t>dataA1_1_4</t>
+  </si>
+  <si>
+    <t>dataA1_1_5</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>dataA1_2_1</t>
+  </si>
+  <si>
+    <t>dataA1_2_2</t>
+  </si>
+  <si>
+    <t>dataA1_2_3</t>
+  </si>
+  <si>
+    <t>dataA1_2_4</t>
+  </si>
+  <si>
+    <t>dataA1_2_5</t>
+  </si>
+  <si>
+    <t>dataA1_3_1</t>
+  </si>
+  <si>
+    <t>dataA1_3_2</t>
+  </si>
+  <si>
+    <t>dataA1_3_3</t>
+  </si>
+  <si>
+    <t>dataA1_3_4</t>
+  </si>
+  <si>
+    <t>dataA1_3_5</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
     <t>DataA2_1</t>
   </si>
   <si>
@@ -82,7 +133,40 @@
     <t>DataA2_4</t>
   </si>
   <si>
-    <t>Runmode Result</t>
+    <t>dataA2_1_1</t>
+  </si>
+  <si>
+    <t>dataA2_1_2</t>
+  </si>
+  <si>
+    <t>dataA2_1_3</t>
+  </si>
+  <si>
+    <t>dataA2_1_4</t>
+  </si>
+  <si>
+    <t>dataA2_2_1</t>
+  </si>
+  <si>
+    <t>dataA2_2_2</t>
+  </si>
+  <si>
+    <t>dataA2_2_3</t>
+  </si>
+  <si>
+    <t>dataA2_2_4</t>
+  </si>
+  <si>
+    <t>dataA2_3_1</t>
+  </si>
+  <si>
+    <t>dataA2_3_2</t>
+  </si>
+  <si>
+    <t>dataA2_3_3</t>
+  </si>
+  <si>
+    <t>dataA2_3_4</t>
   </si>
 </sst>
 </file>
@@ -90,8 +174,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -104,14 +188,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -120,48 +196,102 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,67 +305,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,13 +347,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +455,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,49 +485,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,55 +503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,37 +521,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,16 +560,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,26 +594,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,165 +622,176 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1037,14 +1121,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="44.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="10.7142857142857" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.1428571428571" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.7142857142857" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1061,7 +1146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1072,18 +1157,21 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="D3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1098,17 +1186,18 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="13.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="13.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.4285714285714" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.8571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5714285714286" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.4285714285714" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7142857142857" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1131,40 +1220,82 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8">
@@ -1174,7 +1305,9 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8">
@@ -1184,7 +1317,9 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8">
@@ -1194,7 +1329,9 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8">
@@ -1204,7 +1341,9 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8">
@@ -1214,7 +1353,9 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
   </sheetData>
@@ -1229,57 +1370,102 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="14.4285714285714" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.4285714285714" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.2857142857143" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="7.25714285714286" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7">
@@ -1288,7 +1474,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
@@ -1297,7 +1485,9 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
   </sheetData>

</xml_diff>